<commit_message>
new location coordinates and background
</commit_message>
<xml_diff>
--- a/stimuli_tables/stimuli_demo.xlsx
+++ b/stimuli_tables/stimuli_demo.xlsx
@@ -8,15 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_ALEX_\_Munka\MTA\programming\main_task_online\TerKepEsz_Online\stimuli_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28038F16-F39E-4BCC-8096-492A48CFE879}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE364339-2940-4F7F-BDE6-A6FD31AC3C43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29955" yWindow="1695" windowWidth="19785" windowHeight="11475" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stimuli_demo" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
@@ -500,7 +506,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -572,16 +578,16 @@
         <v>16</v>
       </c>
       <c r="F2">
-        <v>300</v>
+        <v>-375</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>-75</v>
       </c>
       <c r="H2">
-        <v>-300</v>
+        <v>375</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>-75</v>
       </c>
       <c r="J2" t="s">
         <v>17</v>
@@ -610,16 +616,16 @@
         <v>19</v>
       </c>
       <c r="F3">
-        <v>300</v>
+        <v>-375</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>-75</v>
       </c>
       <c r="H3">
-        <v>-300</v>
+        <v>375</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>-75</v>
       </c>
       <c r="J3" t="s">
         <v>17</v>
@@ -648,16 +654,16 @@
         <v>21</v>
       </c>
       <c r="F4">
-        <v>300</v>
+        <v>-375</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>-75</v>
       </c>
       <c r="H4">
-        <v>-300</v>
+        <v>375</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>-75</v>
       </c>
       <c r="J4" t="s">
         <v>17</v>
@@ -686,16 +692,16 @@
         <v>23</v>
       </c>
       <c r="F5">
-        <v>300</v>
+        <v>-375</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>-75</v>
       </c>
       <c r="H5">
-        <v>-300</v>
+        <v>375</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>-75</v>
       </c>
       <c r="J5" t="s">
         <v>24</v>
@@ -724,16 +730,16 @@
         <v>27</v>
       </c>
       <c r="F6">
-        <v>300</v>
+        <v>-375</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>-75</v>
       </c>
       <c r="H6">
-        <v>-300</v>
+        <v>375</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>-75</v>
       </c>
       <c r="J6" t="s">
         <v>17</v>
@@ -762,16 +768,16 @@
         <v>30</v>
       </c>
       <c r="F7">
-        <v>-300</v>
+        <v>-225</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>-75</v>
       </c>
       <c r="H7">
-        <v>-212.13203440000001</v>
+        <v>-225</v>
       </c>
       <c r="I7">
-        <v>-212.13203440000001</v>
+        <v>-225</v>
       </c>
       <c r="J7" t="s">
         <v>31</v>
@@ -800,16 +806,16 @@
         <v>32</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>-375</v>
       </c>
       <c r="G8">
-        <v>300</v>
+        <v>-75</v>
       </c>
       <c r="H8">
-        <v>-212.13203440000001</v>
+        <v>-225</v>
       </c>
       <c r="I8">
-        <v>212.13203440000001</v>
+        <v>-75</v>
       </c>
       <c r="J8" t="s">
         <v>33</v>
@@ -838,16 +844,16 @@
         <v>34</v>
       </c>
       <c r="F9">
-        <v>212.13203440000001</v>
+        <v>-225</v>
       </c>
       <c r="G9">
-        <v>212.13203440000001</v>
+        <v>75</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>-225</v>
       </c>
       <c r="I9">
-        <v>300</v>
+        <v>225</v>
       </c>
       <c r="J9" t="s">
         <v>35</v>
@@ -876,16 +882,16 @@
         <v>20</v>
       </c>
       <c r="F10">
-        <v>300</v>
+        <v>-225</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="H10">
-        <v>-212.13203440000001</v>
+        <v>225</v>
       </c>
       <c r="I10">
-        <v>212.13203440000001</v>
+        <v>-225</v>
       </c>
       <c r="J10" t="s">
         <v>36</v>
@@ -914,16 +920,16 @@
         <v>20</v>
       </c>
       <c r="F11">
-        <v>300</v>
+        <v>-375</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>-75</v>
       </c>
       <c r="H11">
-        <v>-300</v>
+        <v>375</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>-75</v>
       </c>
       <c r="J11" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
fixed coordinate delays + new demo
</commit_message>
<xml_diff>
--- a/stimuli_tables/stimuli_demo.xlsx
+++ b/stimuli_tables/stimuli_demo.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_ALEX_\_Munka\MTA\programming\main_task_online\TerKepEsz_Online\stimuli_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE364339-2940-4F7F-BDE6-A6FD31AC3C43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DD26C3-4B3B-433B-B9E7-373D5E8D3F8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29955" yWindow="1695" windowWidth="19785" windowHeight="11475" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32535" yWindow="3255" windowWidth="22020" windowHeight="11475" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="stimuli_demo" sheetId="1" r:id="rId1"/>
+    <sheet name="stimuli_demo" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="31">
   <si>
     <t>Task</t>
   </si>
@@ -78,21 +78,6 @@
     <t>LURE</t>
   </si>
   <si>
-    <t>stimuli/fractals/149a.jpg</t>
-  </si>
-  <si>
-    <t>stimuli/fractals/149b.jpg</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>stimuli/fractals/181b.jpg</t>
-  </si>
-  <si>
-    <t>stimuli/fractals/181c.jpg</t>
-  </si>
-  <si>
     <t>stimuli/fractals/177b.jpg</t>
   </si>
   <si>
@@ -105,9 +90,6 @@
     <t>stimuli/fractals/167b.jpg</t>
   </si>
   <si>
-    <t>OBJ-TARGET</t>
-  </si>
-  <si>
     <t>FOIL</t>
   </si>
   <si>
@@ -117,34 +99,31 @@
     <t>stimuli/fractals/173c.jpg</t>
   </si>
   <si>
-    <t>Új Képek</t>
-  </si>
-  <si>
     <t>LOC</t>
   </si>
   <si>
     <t>stimuli/fractals/166a.jpg</t>
   </si>
   <si>
-    <t>LOC-TARGET, OBJ-LURE</t>
-  </si>
-  <si>
     <t>stimuli/fractals/159a.jpg</t>
   </si>
   <si>
-    <t>LOC-LURE</t>
-  </si>
-  <si>
     <t>stimuli/fractals/148b.jpg</t>
   </si>
   <si>
-    <t>LOC-FOIL</t>
-  </si>
-  <si>
-    <t>OBJ-LURE</t>
-  </si>
-  <si>
-    <t>Új Helyek</t>
+    <t>TARGET</t>
+  </si>
+  <si>
+    <t>Régi Kép</t>
+  </si>
+  <si>
+    <t>Új Kép</t>
+  </si>
+  <si>
+    <t>Régi Hely</t>
+  </si>
+  <si>
+    <t>Új Hely</t>
   </si>
 </sst>
 </file>
@@ -502,25 +481,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F915FA-A426-4682-8988-FCB7AC529540}">
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="5" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.85546875" customWidth="1"/>
     <col min="8" max="9" width="12.42578125" customWidth="1"/>
     <col min="10" max="10" width="22.85546875" customWidth="1"/>
     <col min="11" max="11" width="14.140625" customWidth="1"/>
     <col min="12" max="12" width="5.5703125" customWidth="1"/>
-    <col min="13" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -569,34 +547,22 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
       <c r="F2">
-        <v>-375</v>
+        <v>-75</v>
       </c>
       <c r="G2">
         <v>-75</v>
       </c>
-      <c r="H2">
-        <v>375</v>
-      </c>
-      <c r="I2">
-        <v>-75</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
       <c r="K2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L2">
-        <v>1000</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -610,31 +576,19 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F3">
-        <v>-375</v>
+        <v>-75</v>
       </c>
       <c r="G3">
         <v>-75</v>
-      </c>
-      <c r="H3">
-        <v>375</v>
-      </c>
-      <c r="I3">
-        <v>-75</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
       </c>
       <c r="K3" t="s">
         <v>28</v>
       </c>
       <c r="L3">
-        <v>2300</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -645,34 +599,22 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F4">
-        <v>-375</v>
+        <v>-75</v>
       </c>
       <c r="G4">
         <v>-75</v>
       </c>
-      <c r="H4">
-        <v>375</v>
-      </c>
-      <c r="I4">
-        <v>-75</v>
-      </c>
-      <c r="J4" t="s">
-        <v>17</v>
-      </c>
       <c r="K4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L4">
-        <v>800</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -685,32 +627,20 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
+      <c r="D5" t="s">
+        <v>18</v>
       </c>
       <c r="F5">
-        <v>-375</v>
+        <v>-75</v>
       </c>
       <c r="G5">
         <v>-75</v>
-      </c>
-      <c r="H5">
-        <v>375</v>
-      </c>
-      <c r="I5">
-        <v>-75</v>
-      </c>
-      <c r="J5" t="s">
-        <v>24</v>
       </c>
       <c r="K5" t="s">
         <v>28</v>
       </c>
       <c r="L5">
-        <v>1500</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -721,34 +651,22 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>-75</v>
+      </c>
+      <c r="G6">
+        <v>-75</v>
+      </c>
+      <c r="K6" t="s">
         <v>27</v>
       </c>
-      <c r="F6">
-        <v>-375</v>
-      </c>
-      <c r="G6">
-        <v>-75</v>
-      </c>
-      <c r="H6">
-        <v>375</v>
-      </c>
-      <c r="I6">
-        <v>-75</v>
-      </c>
-      <c r="J6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" t="s">
-        <v>28</v>
-      </c>
       <c r="L6">
-        <v>600</v>
+        <v>800</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -756,37 +674,25 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" t="s">
-        <v>30</v>
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
       </c>
       <c r="F7">
-        <v>-225</v>
+        <v>-75</v>
       </c>
       <c r="G7">
         <v>-75</v>
       </c>
-      <c r="H7">
-        <v>-225</v>
-      </c>
-      <c r="I7">
-        <v>-225</v>
-      </c>
-      <c r="J7" t="s">
-        <v>31</v>
-      </c>
       <c r="K7" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="L7">
-        <v>800</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -794,37 +700,25 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8">
+        <v>-75</v>
+      </c>
+      <c r="G8">
+        <v>225</v>
+      </c>
+      <c r="K8" t="s">
         <v>29</v>
       </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8">
-        <v>-375</v>
-      </c>
-      <c r="G8">
-        <v>-75</v>
-      </c>
-      <c r="H8">
-        <v>-225</v>
-      </c>
-      <c r="I8">
-        <v>-75</v>
-      </c>
-      <c r="J8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" t="s">
-        <v>37</v>
-      </c>
       <c r="L8">
-        <v>1500</v>
+        <v>800</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -832,37 +726,25 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F9">
         <v>-225</v>
       </c>
       <c r="G9">
-        <v>75</v>
-      </c>
-      <c r="H9">
-        <v>-225</v>
-      </c>
-      <c r="I9">
         <v>225</v>
       </c>
-      <c r="J9" t="s">
-        <v>35</v>
-      </c>
       <c r="K9" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="L9">
-        <v>800</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -870,34 +752,22 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10">
+        <v>-375</v>
+      </c>
+      <c r="G10">
+        <v>225</v>
+      </c>
+      <c r="K10" t="s">
         <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10">
-        <v>-225</v>
-      </c>
-      <c r="G10">
-        <v>75</v>
-      </c>
-      <c r="H10">
-        <v>225</v>
-      </c>
-      <c r="I10">
-        <v>-225</v>
-      </c>
-      <c r="J10" t="s">
-        <v>36</v>
-      </c>
-      <c r="K10" t="s">
-        <v>37</v>
       </c>
       <c r="L10">
         <v>800</v>
@@ -908,45 +778,132 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F11">
         <v>-375</v>
       </c>
       <c r="G11">
-        <v>-75</v>
-      </c>
-      <c r="H11">
-        <v>375</v>
-      </c>
-      <c r="I11">
-        <v>-75</v>
-      </c>
-      <c r="J11" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="K11" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="L11">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <v>-375</v>
+      </c>
+      <c r="G12">
+        <v>225</v>
+      </c>
+      <c r="K12" t="s">
+        <v>29</v>
+      </c>
+      <c r="L12">
         <v>1200</v>
       </c>
     </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13">
+        <v>-75</v>
+      </c>
+      <c r="G13">
+        <v>-225</v>
+      </c>
+      <c r="K13" t="s">
+        <v>30</v>
+      </c>
+      <c r="L13">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14">
+        <v>225</v>
+      </c>
+      <c r="G14">
+        <v>-75</v>
+      </c>
+      <c r="K14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L14">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15">
+        <v>-225</v>
+      </c>
+      <c r="G15">
+        <v>225</v>
+      </c>
+      <c r="K15" t="s">
+        <v>30</v>
+      </c>
+      <c r="L15">
+        <v>800</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>